<commit_message>
remove "s" from sheet/column names
</commit_message>
<xml_diff>
--- a/data/data_files/double_perovskites.xlsx
+++ b/data/data_files/double_perovskites.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alirezafaghaninia/Documents/py3/py3_codes/matbench/data/data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD4CAD38-5881-0547-8717-598DFE71D2F8}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{54DCCA42-C7C7-E248-B530-76DDEDB421CE}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4360" yWindow="460" windowWidth="27560" windowHeight="21200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="gaps" sheetId="1" r:id="rId1"/>
+    <sheet name="bandgap" sheetId="1" r:id="rId1"/>
     <sheet name="lumo" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>

</xml_diff>